<commit_message>
Update project rubric, add DailyScrum notes
</commit_message>
<xml_diff>
--- a/ProjectRubric1of4.xlsx
+++ b/ProjectRubric1of4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elari\Desktop\Harvard\CSCI_S71\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elari\Documents\Repos\CSCI_S71\Teamify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D761BD-B881-4453-AD17-8C8C8F7CCAB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3835483B-26BD-43FB-91AD-025E174039BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{240F924D-48B8-43CB-A5F6-3B6DFA99720D}"/>
+    <workbookView xWindow="18660" yWindow="-15555" windowWidth="17415" windowHeight="13065" xr2:uid="{240F924D-48B8-43CB-A5F6-3B6DFA99720D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -170,7 +170,7 @@
     <t>Deferred per Richard's instructions in Slack channel #summer2020.  See above</t>
   </si>
   <si>
-    <t>The repository is created but has not yet been submitted as the solution.  Each team member will perform an Assigment submission individually.</t>
+    <t xml:space="preserve">The repository is created but has not yet been submitted as the solution.  Each team member will perform an Assignment submission individually pending a response from Richard to Michael's inquiry on Slack.  The team developed an assignment submission together that Eric will post 6/28/20.    </t>
   </si>
 </sst>
 </file>
@@ -260,18 +260,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -285,7 +278,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -602,10 +595,10 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -675,7 +668,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
@@ -850,7 +843,10 @@
         <v>4</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>34</v>
+        <v>7</v>
+      </c>
+      <c r="E16" s="3">
+        <v>44010</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>41</v>
@@ -960,10 +956,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">

</xml_diff>